<commit_message>
update benchmarking of new risk group for px
</commit_message>
<xml_diff>
--- a/data/table_significant_cpgs_OS_EFS_summary.xlsx
+++ b/data/table_significant_cpgs_OS_EFS_summary.xlsx
@@ -14,21 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Significant CpG probes in EFS</t>
+  </si>
   <si>
     <t>Significant CpG probes in OS</t>
-  </si>
-  <si>
-    <t>Significant CpG probes in EFS</t>
   </si>
   <si>
     <t>Significant overlapping CpG probes</t>
   </si>
   <si>
-    <t>Unadjusted</t>
-  </si>
-  <si>
-    <t>Adjusted</t>
+    <t>Updated Risk Group</t>
   </si>
 </sst>
 </file>
@@ -386,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,26 +405,12 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3740</v>
+        <v>112</v>
       </c>
       <c r="C2">
-        <v>2634</v>
+        <v>189</v>
       </c>
       <c r="D2">
-        <v>1741</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>167</v>
-      </c>
-      <c r="C3">
-        <v>55</v>
-      </c>
-      <c r="D3">
         <v>17</v>
       </c>
     </row>

</xml_diff>